<commit_message>
Vocabulary Update & ANKI-File added
</commit_message>
<xml_diff>
--- a/vokabeln.xlsx
+++ b/vokabeln.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\0-Rumänisch\own\romanian_vocab_anki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C5226-94D8-4D8A-859C-2662D5BF5E8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE7712D-EDC3-4E8A-AB2B-ABDF467A4D2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20052" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{36CC22FB-63D4-41CD-AB8B-40A978F9033C}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8807" uniqueCount="5815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8884" uniqueCount="5827">
   <si>
     <t>DE</t>
   </si>
@@ -17511,6 +17511,42 @@
   </si>
   <si>
     <t>beri</t>
+  </si>
+  <si>
+    <t>frigider</t>
+  </si>
+  <si>
+    <t>Kühlschrank</t>
+  </si>
+  <si>
+    <t>frigidere</t>
+  </si>
+  <si>
+    <t>atrăgător</t>
+  </si>
+  <si>
+    <t>attraktiv</t>
+  </si>
+  <si>
+    <t>atrăgătoare</t>
+  </si>
+  <si>
+    <t>reci</t>
+  </si>
+  <si>
+    <t>iute</t>
+  </si>
+  <si>
+    <t>scharf (gwürzt)</t>
+  </si>
+  <si>
+    <t>iuți</t>
+  </si>
+  <si>
+    <t>cumsecade</t>
+  </si>
+  <si>
+    <t>anständig</t>
   </si>
 </sst>
 </file>
@@ -18083,7 +18119,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J142" sqref="A2:J142"/>
+      <selection pane="bottomLeft" activeCell="I149" sqref="A2:I149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22058,16 +22094,40 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>5816</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5815</v>
+      </c>
+      <c r="C143" t="s">
+        <v>5817</v>
+      </c>
+      <c r="F143" s="14" t="s">
+        <v>80</v>
+      </c>
       <c r="G143" s="5" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>un</v>
       </c>
       <c r="H143" s="4" t="str">
         <f t="shared" si="8"/>
-        <v/>
+        <v>două</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>5819</v>
+      </c>
+      <c r="B144" t="s">
+        <v>5818</v>
+      </c>
+      <c r="C144" t="s">
+        <v>5820</v>
+      </c>
+      <c r="F144" s="14" t="s">
+        <v>5786</v>
+      </c>
       <c r="G144" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22077,7 +22137,19 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C145" t="s">
+        <v>5821</v>
+      </c>
+      <c r="F145" s="14" t="s">
+        <v>5786</v>
+      </c>
       <c r="G145" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22087,7 +22159,19 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>904</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C146" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F146" s="14" t="s">
+        <v>5786</v>
+      </c>
       <c r="G146" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22097,7 +22181,19 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B147" t="s">
+        <v>542</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2989</v>
+      </c>
+      <c r="F147" s="14" t="s">
+        <v>5786</v>
+      </c>
       <c r="G147" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22107,7 +22203,19 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>5823</v>
+      </c>
+      <c r="B148" t="s">
+        <v>5822</v>
+      </c>
+      <c r="C148" t="s">
+        <v>5824</v>
+      </c>
+      <c r="F148" s="14" t="s">
+        <v>5786</v>
+      </c>
       <c r="G148" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22117,7 +22225,19 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>5826</v>
+      </c>
+      <c r="B149" t="s">
+        <v>5825</v>
+      </c>
+      <c r="C149" t="s">
+        <v>5825</v>
+      </c>
+      <c r="F149" s="14" t="s">
+        <v>5786</v>
+      </c>
       <c r="G149" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22127,7 +22247,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G150" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22137,7 +22257,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G151" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22147,7 +22267,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G152" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22157,7 +22277,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G153" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22167,7 +22287,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G154" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22177,7 +22297,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G155" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22187,7 +22307,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G156" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22197,7 +22317,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G157" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22207,7 +22327,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G158" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22217,7 +22337,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G159" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -22227,7 +22347,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G160" s="5" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -54236,10 +54356,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1BFFFA-3DE2-4CFE-BE80-A950A2B6A0C1}">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:J148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="G146" sqref="G146"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57642,6 +57762,167 @@
         <v>5580</v>
       </c>
     </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>5816</v>
+      </c>
+      <c r="B142" t="s">
+        <v>5815</v>
+      </c>
+      <c r="C142" t="s">
+        <v>5817</v>
+      </c>
+      <c r="F142" t="s">
+        <v>80</v>
+      </c>
+      <c r="G142" t="s">
+        <v>318</v>
+      </c>
+      <c r="H142" t="s">
+        <v>615</v>
+      </c>
+      <c r="I142" t="s">
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>5819</v>
+      </c>
+      <c r="B143" t="s">
+        <v>5818</v>
+      </c>
+      <c r="C143" t="s">
+        <v>5820</v>
+      </c>
+      <c r="F143" t="s">
+        <v>5786</v>
+      </c>
+      <c r="G143" t="s">
+        <v>5782</v>
+      </c>
+      <c r="H143" t="s">
+        <v>5782</v>
+      </c>
+      <c r="I143" t="s">
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>3310</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C144" t="s">
+        <v>5821</v>
+      </c>
+      <c r="F144" t="s">
+        <v>5786</v>
+      </c>
+      <c r="G144" t="s">
+        <v>5782</v>
+      </c>
+      <c r="H144" t="s">
+        <v>5782</v>
+      </c>
+      <c r="I144" t="s">
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>904</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C145" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F145" t="s">
+        <v>5786</v>
+      </c>
+      <c r="G145" t="s">
+        <v>5782</v>
+      </c>
+      <c r="H145" t="s">
+        <v>5782</v>
+      </c>
+      <c r="I145" t="s">
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B146" t="s">
+        <v>542</v>
+      </c>
+      <c r="C146" t="s">
+        <v>2989</v>
+      </c>
+      <c r="F146" t="s">
+        <v>5786</v>
+      </c>
+      <c r="G146" t="s">
+        <v>5782</v>
+      </c>
+      <c r="H146" t="s">
+        <v>5782</v>
+      </c>
+      <c r="I146" t="s">
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>5823</v>
+      </c>
+      <c r="B147" t="s">
+        <v>5822</v>
+      </c>
+      <c r="C147" t="s">
+        <v>5824</v>
+      </c>
+      <c r="F147" t="s">
+        <v>5786</v>
+      </c>
+      <c r="G147" t="s">
+        <v>5782</v>
+      </c>
+      <c r="H147" t="s">
+        <v>5782</v>
+      </c>
+      <c r="I147" t="s">
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>5826</v>
+      </c>
+      <c r="B148" t="s">
+        <v>5825</v>
+      </c>
+      <c r="C148" t="s">
+        <v>5825</v>
+      </c>
+      <c r="F148" t="s">
+        <v>5786</v>
+      </c>
+      <c r="G148" t="s">
+        <v>5782</v>
+      </c>
+      <c r="H148" t="s">
+        <v>5782</v>
+      </c>
+      <c r="I148" t="s">
+        <v>5580</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>